<commit_message>
Added example territories for three companies in NY
</commit_message>
<xml_diff>
--- a/references_public/allstate_roc.xlsx
+++ b/references_public/allstate_roc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevin/Source/geospatial_rating/references_public/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C16B5B6B-BA3F-2541-A511-260A836693CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{275D1324-114E-A740-9CAF-B2CD31C56BC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="29740" activeTab="3" xr2:uid="{214689B6-D7E3-F549-9D27-565D3B501068}"/>
+    <workbookView xWindow="31660" yWindow="21100" windowWidth="38400" windowHeight="29740" activeTab="3" xr2:uid="{214689B6-D7E3-F549-9D27-565D3B501068}"/>
   </bookViews>
   <sheets>
     <sheet name="Complete" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4701" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4702" uniqueCount="164">
   <si>
     <t>PREMIUM CALCULATION STEP</t>
   </si>
@@ -551,6 +551,9 @@
   </si>
   <si>
     <t>SERFF #ESUR-129739117</t>
+  </si>
+  <si>
+    <t>Hurricane in NY</t>
   </si>
 </sst>
 </file>
@@ -1261,10 +1264,39 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1282,18 +1314,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1309,23 +1329,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1687,28 +1690,28 @@
     </row>
     <row r="2" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B3" s="112" t="s">
+      <c r="B3" s="125" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="113"/>
-      <c r="D3" s="109" t="s">
+      <c r="C3" s="126"/>
+      <c r="D3" s="123" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="110"/>
-      <c r="F3" s="110"/>
-      <c r="G3" s="110"/>
-      <c r="H3" s="110"/>
-      <c r="I3" s="110"/>
-      <c r="J3" s="110"/>
-      <c r="K3" s="110"/>
-      <c r="L3" s="110"/>
-      <c r="M3" s="110"/>
-      <c r="N3" s="110"/>
-      <c r="O3" s="111"/>
+      <c r="E3" s="118"/>
+      <c r="F3" s="118"/>
+      <c r="G3" s="118"/>
+      <c r="H3" s="118"/>
+      <c r="I3" s="118"/>
+      <c r="J3" s="118"/>
+      <c r="K3" s="118"/>
+      <c r="L3" s="118"/>
+      <c r="M3" s="118"/>
+      <c r="N3" s="118"/>
+      <c r="O3" s="124"/>
     </row>
     <row r="4" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="114"/>
-      <c r="C4" s="115"/>
+      <c r="B4" s="127"/>
+      <c r="C4" s="128"/>
       <c r="D4" s="23">
         <v>1</v>
       </c>
@@ -3614,46 +3617,46 @@
     </row>
     <row r="47" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="48" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="116" t="s">
+      <c r="B48" s="119" t="s">
         <v>47</v>
       </c>
-      <c r="C48" s="117"/>
-      <c r="D48" s="117"/>
-      <c r="E48" s="117"/>
-      <c r="F48" s="117"/>
-      <c r="G48" s="117"/>
-      <c r="H48" s="117"/>
-      <c r="I48" s="117"/>
-      <c r="J48" s="117"/>
-      <c r="K48" s="117"/>
-      <c r="L48" s="117"/>
-      <c r="M48" s="117"/>
-      <c r="N48" s="117"/>
-      <c r="O48" s="118"/>
+      <c r="C48" s="120"/>
+      <c r="D48" s="120"/>
+      <c r="E48" s="120"/>
+      <c r="F48" s="120"/>
+      <c r="G48" s="120"/>
+      <c r="H48" s="120"/>
+      <c r="I48" s="120"/>
+      <c r="J48" s="120"/>
+      <c r="K48" s="120"/>
+      <c r="L48" s="120"/>
+      <c r="M48" s="120"/>
+      <c r="N48" s="120"/>
+      <c r="O48" s="121"/>
     </row>
     <row r="49" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B49" s="112" t="s">
+      <c r="B49" s="125" t="s">
         <v>0</v>
       </c>
-      <c r="C49" s="113"/>
-      <c r="D49" s="109" t="s">
+      <c r="C49" s="126"/>
+      <c r="D49" s="123" t="s">
         <v>4</v>
       </c>
-      <c r="E49" s="110"/>
-      <c r="F49" s="110"/>
-      <c r="G49" s="110"/>
-      <c r="H49" s="110"/>
-      <c r="I49" s="110"/>
-      <c r="J49" s="110"/>
-      <c r="K49" s="110"/>
-      <c r="L49" s="110"/>
-      <c r="M49" s="110"/>
-      <c r="N49" s="110"/>
-      <c r="O49" s="111"/>
+      <c r="E49" s="118"/>
+      <c r="F49" s="118"/>
+      <c r="G49" s="118"/>
+      <c r="H49" s="118"/>
+      <c r="I49" s="118"/>
+      <c r="J49" s="118"/>
+      <c r="K49" s="118"/>
+      <c r="L49" s="118"/>
+      <c r="M49" s="118"/>
+      <c r="N49" s="118"/>
+      <c r="O49" s="124"/>
     </row>
     <row r="50" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="114"/>
-      <c r="C50" s="115"/>
+      <c r="B50" s="127"/>
+      <c r="C50" s="128"/>
       <c r="D50" s="23">
         <v>1</v>
       </c>
@@ -4317,11 +4320,11 @@
     </row>
     <row r="72" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="73" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="116" t="s">
+      <c r="B73" s="119" t="s">
         <v>61</v>
       </c>
-      <c r="C73" s="117"/>
-      <c r="D73" s="118"/>
+      <c r="C73" s="120"/>
+      <c r="D73" s="121"/>
     </row>
     <row r="74" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B74" s="15">
@@ -4443,11 +4446,11 @@
       </c>
     </row>
     <row r="85" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B85" s="119" t="s">
+      <c r="B85" s="122" t="s">
         <v>62</v>
       </c>
-      <c r="C85" s="119"/>
-      <c r="D85" s="119"/>
+      <c r="C85" s="122"/>
+      <c r="D85" s="122"/>
     </row>
     <row r="86" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="87" spans="2:4" x14ac:dyDescent="0.2">
@@ -4527,11 +4530,11 @@
     </row>
     <row r="94" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="95" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B95" s="109" t="s">
+      <c r="B95" s="123" t="s">
         <v>80</v>
       </c>
-      <c r="C95" s="110"/>
-      <c r="D95" s="111"/>
+      <c r="C95" s="118"/>
+      <c r="D95" s="124"/>
     </row>
     <row r="96" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B96" s="15">
@@ -4598,19 +4601,19 @@
       </c>
     </row>
     <row r="102" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B102" s="110" t="s">
+      <c r="B102" s="118" t="s">
         <v>86</v>
       </c>
-      <c r="C102" s="110"/>
-      <c r="D102" s="110"/>
+      <c r="C102" s="118"/>
+      <c r="D102" s="118"/>
     </row>
     <row r="103" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="104" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B104" s="109" t="s">
+      <c r="B104" s="123" t="s">
         <v>88</v>
       </c>
-      <c r="C104" s="110"/>
-      <c r="D104" s="111"/>
+      <c r="C104" s="118"/>
+      <c r="D104" s="124"/>
     </row>
     <row r="105" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B105" s="15">
@@ -4667,11 +4670,11 @@
     </row>
     <row r="110" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="111" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B111" s="109" t="s">
+      <c r="B111" s="123" t="s">
         <v>93</v>
       </c>
-      <c r="C111" s="110"/>
-      <c r="D111" s="111"/>
+      <c r="C111" s="118"/>
+      <c r="D111" s="124"/>
     </row>
     <row r="112" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B112" s="15">
@@ -4738,19 +4741,19 @@
       </c>
     </row>
     <row r="118" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B118" s="110" t="s">
+      <c r="B118" s="118" t="s">
         <v>99</v>
       </c>
-      <c r="C118" s="110"/>
-      <c r="D118" s="110"/>
+      <c r="C118" s="118"/>
+      <c r="D118" s="118"/>
     </row>
     <row r="119" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="120" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B120" s="116" t="s">
+      <c r="B120" s="119" t="s">
         <v>100</v>
       </c>
-      <c r="C120" s="117"/>
-      <c r="D120" s="118"/>
+      <c r="C120" s="120"/>
+      <c r="D120" s="121"/>
     </row>
     <row r="121" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B121" s="15">
@@ -5005,11 +5008,11 @@
     </row>
     <row r="144" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="145" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B145" s="116" t="s">
+      <c r="B145" s="119" t="s">
         <v>124</v>
       </c>
-      <c r="C145" s="117"/>
-      <c r="D145" s="118"/>
+      <c r="C145" s="120"/>
+      <c r="D145" s="121"/>
     </row>
     <row r="146" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B146" s="15">
@@ -5055,11 +5058,11 @@
     </row>
     <row r="150" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="151" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B151" s="116" t="s">
+      <c r="B151" s="119" t="s">
         <v>128</v>
       </c>
-      <c r="C151" s="117"/>
-      <c r="D151" s="118"/>
+      <c r="C151" s="120"/>
+      <c r="D151" s="121"/>
     </row>
     <row r="152" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B152" s="15">
@@ -5093,6 +5096,11 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="D3:O3"/>
+    <mergeCell ref="B3:C4"/>
+    <mergeCell ref="B49:C50"/>
+    <mergeCell ref="D49:O49"/>
+    <mergeCell ref="B48:O48"/>
     <mergeCell ref="B118:D118"/>
     <mergeCell ref="B120:D120"/>
     <mergeCell ref="B145:D145"/>
@@ -5103,11 +5111,6 @@
     <mergeCell ref="B102:D102"/>
     <mergeCell ref="B104:D104"/>
     <mergeCell ref="B111:D111"/>
-    <mergeCell ref="D3:O3"/>
-    <mergeCell ref="B3:C4"/>
-    <mergeCell ref="B49:C50"/>
-    <mergeCell ref="D49:O49"/>
-    <mergeCell ref="B48:O48"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5138,28 +5141,28 @@
     </row>
     <row r="2" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B3" s="112" t="s">
+      <c r="B3" s="125" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="113"/>
-      <c r="D3" s="109" t="s">
+      <c r="C3" s="126"/>
+      <c r="D3" s="123" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="110"/>
-      <c r="F3" s="110"/>
-      <c r="G3" s="110"/>
-      <c r="H3" s="110"/>
-      <c r="I3" s="110"/>
-      <c r="J3" s="110"/>
-      <c r="K3" s="110"/>
-      <c r="L3" s="110"/>
-      <c r="M3" s="110"/>
-      <c r="N3" s="110"/>
-      <c r="O3" s="111"/>
+      <c r="E3" s="118"/>
+      <c r="F3" s="118"/>
+      <c r="G3" s="118"/>
+      <c r="H3" s="118"/>
+      <c r="I3" s="118"/>
+      <c r="J3" s="118"/>
+      <c r="K3" s="118"/>
+      <c r="L3" s="118"/>
+      <c r="M3" s="118"/>
+      <c r="N3" s="118"/>
+      <c r="O3" s="124"/>
     </row>
     <row r="4" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="114"/>
-      <c r="C4" s="115"/>
+      <c r="B4" s="127"/>
+      <c r="C4" s="128"/>
       <c r="D4" s="23">
         <v>1</v>
       </c>
@@ -7065,46 +7068,46 @@
     </row>
     <row r="47" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="48" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="116" t="s">
+      <c r="B48" s="119" t="s">
         <v>47</v>
       </c>
-      <c r="C48" s="117"/>
-      <c r="D48" s="117"/>
-      <c r="E48" s="117"/>
-      <c r="F48" s="117"/>
-      <c r="G48" s="117"/>
-      <c r="H48" s="117"/>
-      <c r="I48" s="117"/>
-      <c r="J48" s="117"/>
-      <c r="K48" s="117"/>
-      <c r="L48" s="117"/>
-      <c r="M48" s="117"/>
-      <c r="N48" s="117"/>
-      <c r="O48" s="118"/>
+      <c r="C48" s="120"/>
+      <c r="D48" s="120"/>
+      <c r="E48" s="120"/>
+      <c r="F48" s="120"/>
+      <c r="G48" s="120"/>
+      <c r="H48" s="120"/>
+      <c r="I48" s="120"/>
+      <c r="J48" s="120"/>
+      <c r="K48" s="120"/>
+      <c r="L48" s="120"/>
+      <c r="M48" s="120"/>
+      <c r="N48" s="120"/>
+      <c r="O48" s="121"/>
     </row>
     <row r="49" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B49" s="112" t="s">
+      <c r="B49" s="125" t="s">
         <v>0</v>
       </c>
-      <c r="C49" s="113"/>
-      <c r="D49" s="109" t="s">
+      <c r="C49" s="126"/>
+      <c r="D49" s="123" t="s">
         <v>4</v>
       </c>
-      <c r="E49" s="110"/>
-      <c r="F49" s="110"/>
-      <c r="G49" s="110"/>
-      <c r="H49" s="110"/>
-      <c r="I49" s="110"/>
-      <c r="J49" s="110"/>
-      <c r="K49" s="110"/>
-      <c r="L49" s="110"/>
-      <c r="M49" s="110"/>
-      <c r="N49" s="110"/>
-      <c r="O49" s="111"/>
+      <c r="E49" s="118"/>
+      <c r="F49" s="118"/>
+      <c r="G49" s="118"/>
+      <c r="H49" s="118"/>
+      <c r="I49" s="118"/>
+      <c r="J49" s="118"/>
+      <c r="K49" s="118"/>
+      <c r="L49" s="118"/>
+      <c r="M49" s="118"/>
+      <c r="N49" s="118"/>
+      <c r="O49" s="124"/>
     </row>
     <row r="50" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="114"/>
-      <c r="C50" s="115"/>
+      <c r="B50" s="127"/>
+      <c r="C50" s="128"/>
       <c r="D50" s="23">
         <v>1</v>
       </c>
@@ -7768,11 +7771,11 @@
     </row>
     <row r="72" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="73" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="116" t="s">
+      <c r="B73" s="119" t="s">
         <v>61</v>
       </c>
-      <c r="C73" s="117"/>
-      <c r="D73" s="118"/>
+      <c r="C73" s="120"/>
+      <c r="D73" s="121"/>
     </row>
     <row r="74" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B74" s="57">
@@ -7894,11 +7897,11 @@
       </c>
     </row>
     <row r="85" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B85" s="119" t="s">
+      <c r="B85" s="122" t="s">
         <v>62</v>
       </c>
-      <c r="C85" s="119"/>
-      <c r="D85" s="119"/>
+      <c r="C85" s="122"/>
+      <c r="D85" s="122"/>
     </row>
     <row r="86" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="87" spans="2:4" x14ac:dyDescent="0.2">
@@ -7978,11 +7981,11 @@
     </row>
     <row r="94" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="95" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B95" s="109" t="s">
+      <c r="B95" s="123" t="s">
         <v>80</v>
       </c>
-      <c r="C95" s="110"/>
-      <c r="D95" s="111"/>
+      <c r="C95" s="118"/>
+      <c r="D95" s="124"/>
     </row>
     <row r="96" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B96" s="57">
@@ -8049,19 +8052,19 @@
       </c>
     </row>
     <row r="102" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B102" s="110" t="s">
+      <c r="B102" s="118" t="s">
         <v>86</v>
       </c>
-      <c r="C102" s="110"/>
-      <c r="D102" s="110"/>
+      <c r="C102" s="118"/>
+      <c r="D102" s="118"/>
     </row>
     <row r="103" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="104" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B104" s="109" t="s">
+      <c r="B104" s="123" t="s">
         <v>88</v>
       </c>
-      <c r="C104" s="110"/>
-      <c r="D104" s="111"/>
+      <c r="C104" s="118"/>
+      <c r="D104" s="124"/>
     </row>
     <row r="105" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B105" s="57">
@@ -8118,11 +8121,11 @@
     </row>
     <row r="110" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="111" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B111" s="109" t="s">
+      <c r="B111" s="123" t="s">
         <v>93</v>
       </c>
-      <c r="C111" s="110"/>
-      <c r="D111" s="111"/>
+      <c r="C111" s="118"/>
+      <c r="D111" s="124"/>
     </row>
     <row r="112" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B112" s="57">
@@ -8189,19 +8192,19 @@
       </c>
     </row>
     <row r="118" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B118" s="110" t="s">
+      <c r="B118" s="118" t="s">
         <v>99</v>
       </c>
-      <c r="C118" s="110"/>
-      <c r="D118" s="110"/>
+      <c r="C118" s="118"/>
+      <c r="D118" s="118"/>
     </row>
     <row r="119" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="120" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B120" s="116" t="s">
+      <c r="B120" s="119" t="s">
         <v>100</v>
       </c>
-      <c r="C120" s="117"/>
-      <c r="D120" s="118"/>
+      <c r="C120" s="120"/>
+      <c r="D120" s="121"/>
     </row>
     <row r="121" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B121" s="57">
@@ -8456,11 +8459,11 @@
     </row>
     <row r="144" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="145" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B145" s="116" t="s">
+      <c r="B145" s="119" t="s">
         <v>124</v>
       </c>
-      <c r="C145" s="117"/>
-      <c r="D145" s="118"/>
+      <c r="C145" s="120"/>
+      <c r="D145" s="121"/>
     </row>
     <row r="146" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B146" s="57">
@@ -8506,11 +8509,11 @@
     </row>
     <row r="150" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="151" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B151" s="116" t="s">
+      <c r="B151" s="119" t="s">
         <v>128</v>
       </c>
-      <c r="C151" s="117"/>
-      <c r="D151" s="118"/>
+      <c r="C151" s="120"/>
+      <c r="D151" s="121"/>
     </row>
     <row r="152" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B152" s="57">
@@ -8544,12 +8547,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B73:D73"/>
-    <mergeCell ref="B3:C4"/>
-    <mergeCell ref="D3:O3"/>
-    <mergeCell ref="B48:O48"/>
-    <mergeCell ref="B49:C50"/>
-    <mergeCell ref="D49:O49"/>
     <mergeCell ref="B120:D120"/>
     <mergeCell ref="B145:D145"/>
     <mergeCell ref="B151:D151"/>
@@ -8559,6 +8556,12 @@
     <mergeCell ref="B104:D104"/>
     <mergeCell ref="B111:D111"/>
     <mergeCell ref="B118:D118"/>
+    <mergeCell ref="B73:D73"/>
+    <mergeCell ref="B3:C4"/>
+    <mergeCell ref="D3:O3"/>
+    <mergeCell ref="B48:O48"/>
+    <mergeCell ref="B49:C50"/>
+    <mergeCell ref="D49:O49"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -8589,28 +8592,28 @@
     </row>
     <row r="2" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B3" s="112" t="s">
+      <c r="B3" s="125" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="113"/>
-      <c r="D3" s="120" t="s">
+      <c r="C3" s="126"/>
+      <c r="D3" s="129" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="121"/>
-      <c r="F3" s="121"/>
-      <c r="G3" s="121"/>
-      <c r="H3" s="121"/>
-      <c r="I3" s="121"/>
-      <c r="J3" s="121"/>
-      <c r="K3" s="121"/>
-      <c r="L3" s="121"/>
-      <c r="M3" s="121"/>
-      <c r="N3" s="121"/>
-      <c r="O3" s="122"/>
+      <c r="E3" s="130"/>
+      <c r="F3" s="130"/>
+      <c r="G3" s="130"/>
+      <c r="H3" s="130"/>
+      <c r="I3" s="130"/>
+      <c r="J3" s="130"/>
+      <c r="K3" s="130"/>
+      <c r="L3" s="130"/>
+      <c r="M3" s="130"/>
+      <c r="N3" s="130"/>
+      <c r="O3" s="131"/>
     </row>
     <row r="4" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="114"/>
-      <c r="C4" s="115"/>
+      <c r="B4" s="127"/>
+      <c r="C4" s="128"/>
       <c r="D4" s="67">
         <v>1</v>
       </c>
@@ -10516,46 +10519,46 @@
     </row>
     <row r="47" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="48" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="116" t="s">
+      <c r="B48" s="119" t="s">
         <v>47</v>
       </c>
-      <c r="C48" s="117"/>
-      <c r="D48" s="117"/>
-      <c r="E48" s="117"/>
-      <c r="F48" s="117"/>
-      <c r="G48" s="117"/>
-      <c r="H48" s="117"/>
-      <c r="I48" s="117"/>
-      <c r="J48" s="117"/>
-      <c r="K48" s="117"/>
-      <c r="L48" s="117"/>
-      <c r="M48" s="117"/>
-      <c r="N48" s="117"/>
-      <c r="O48" s="118"/>
+      <c r="C48" s="120"/>
+      <c r="D48" s="120"/>
+      <c r="E48" s="120"/>
+      <c r="F48" s="120"/>
+      <c r="G48" s="120"/>
+      <c r="H48" s="120"/>
+      <c r="I48" s="120"/>
+      <c r="J48" s="120"/>
+      <c r="K48" s="120"/>
+      <c r="L48" s="120"/>
+      <c r="M48" s="120"/>
+      <c r="N48" s="120"/>
+      <c r="O48" s="121"/>
     </row>
     <row r="49" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B49" s="112" t="s">
+      <c r="B49" s="125" t="s">
         <v>0</v>
       </c>
-      <c r="C49" s="113"/>
-      <c r="D49" s="120" t="s">
+      <c r="C49" s="126"/>
+      <c r="D49" s="129" t="s">
         <v>4</v>
       </c>
-      <c r="E49" s="121"/>
-      <c r="F49" s="121"/>
-      <c r="G49" s="121"/>
-      <c r="H49" s="121"/>
-      <c r="I49" s="121"/>
-      <c r="J49" s="121"/>
-      <c r="K49" s="121"/>
-      <c r="L49" s="121"/>
-      <c r="M49" s="121"/>
-      <c r="N49" s="121"/>
-      <c r="O49" s="122"/>
+      <c r="E49" s="130"/>
+      <c r="F49" s="130"/>
+      <c r="G49" s="130"/>
+      <c r="H49" s="130"/>
+      <c r="I49" s="130"/>
+      <c r="J49" s="130"/>
+      <c r="K49" s="130"/>
+      <c r="L49" s="130"/>
+      <c r="M49" s="130"/>
+      <c r="N49" s="130"/>
+      <c r="O49" s="131"/>
     </row>
     <row r="50" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="114"/>
-      <c r="C50" s="115"/>
+      <c r="B50" s="127"/>
+      <c r="C50" s="128"/>
       <c r="D50" s="67">
         <v>1</v>
       </c>
@@ -11219,11 +11222,11 @@
     </row>
     <row r="72" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="73" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="116" t="s">
+      <c r="B73" s="119" t="s">
         <v>61</v>
       </c>
-      <c r="C73" s="117"/>
-      <c r="D73" s="118"/>
+      <c r="C73" s="120"/>
+      <c r="D73" s="121"/>
     </row>
     <row r="74" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B74" s="15">
@@ -11345,11 +11348,11 @@
       </c>
     </row>
     <row r="85" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B85" s="119" t="s">
+      <c r="B85" s="122" t="s">
         <v>62</v>
       </c>
-      <c r="C85" s="119"/>
-      <c r="D85" s="119"/>
+      <c r="C85" s="122"/>
+      <c r="D85" s="122"/>
     </row>
     <row r="86" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="87" spans="2:4" x14ac:dyDescent="0.2">
@@ -11429,11 +11432,11 @@
     </row>
     <row r="94" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="95" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B95" s="109" t="s">
+      <c r="B95" s="123" t="s">
         <v>80</v>
       </c>
-      <c r="C95" s="110"/>
-      <c r="D95" s="111"/>
+      <c r="C95" s="118"/>
+      <c r="D95" s="124"/>
     </row>
     <row r="96" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B96" s="15">
@@ -11500,19 +11503,19 @@
       </c>
     </row>
     <row r="102" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B102" s="110" t="s">
+      <c r="B102" s="118" t="s">
         <v>86</v>
       </c>
-      <c r="C102" s="110"/>
-      <c r="D102" s="110"/>
+      <c r="C102" s="118"/>
+      <c r="D102" s="118"/>
     </row>
     <row r="103" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="104" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B104" s="109" t="s">
+      <c r="B104" s="123" t="s">
         <v>88</v>
       </c>
-      <c r="C104" s="110"/>
-      <c r="D104" s="111"/>
+      <c r="C104" s="118"/>
+      <c r="D104" s="124"/>
     </row>
     <row r="105" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B105" s="15">
@@ -11569,11 +11572,11 @@
     </row>
     <row r="110" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="111" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B111" s="109" t="s">
+      <c r="B111" s="123" t="s">
         <v>93</v>
       </c>
-      <c r="C111" s="110"/>
-      <c r="D111" s="111"/>
+      <c r="C111" s="118"/>
+      <c r="D111" s="124"/>
     </row>
     <row r="112" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B112" s="15">
@@ -11640,19 +11643,19 @@
       </c>
     </row>
     <row r="118" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B118" s="110" t="s">
+      <c r="B118" s="118" t="s">
         <v>99</v>
       </c>
-      <c r="C118" s="110"/>
-      <c r="D118" s="110"/>
+      <c r="C118" s="118"/>
+      <c r="D118" s="118"/>
     </row>
     <row r="119" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="120" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B120" s="116" t="s">
+      <c r="B120" s="119" t="s">
         <v>100</v>
       </c>
-      <c r="C120" s="117"/>
-      <c r="D120" s="118"/>
+      <c r="C120" s="120"/>
+      <c r="D120" s="121"/>
     </row>
     <row r="121" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B121" s="15">
@@ -11907,11 +11910,11 @@
     </row>
     <row r="144" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="145" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B145" s="116" t="s">
+      <c r="B145" s="119" t="s">
         <v>124</v>
       </c>
-      <c r="C145" s="117"/>
-      <c r="D145" s="118"/>
+      <c r="C145" s="120"/>
+      <c r="D145" s="121"/>
     </row>
     <row r="146" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B146" s="15">
@@ -11957,11 +11960,11 @@
     </row>
     <row r="150" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="151" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B151" s="116" t="s">
+      <c r="B151" s="119" t="s">
         <v>128</v>
       </c>
-      <c r="C151" s="117"/>
-      <c r="D151" s="118"/>
+      <c r="C151" s="120"/>
+      <c r="D151" s="121"/>
     </row>
     <row r="152" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B152" s="15">
@@ -11995,12 +11998,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B73:D73"/>
-    <mergeCell ref="B3:C4"/>
-    <mergeCell ref="D3:O3"/>
-    <mergeCell ref="B48:O48"/>
-    <mergeCell ref="B49:C50"/>
-    <mergeCell ref="D49:O49"/>
     <mergeCell ref="B120:D120"/>
     <mergeCell ref="B145:D145"/>
     <mergeCell ref="B151:D151"/>
@@ -12010,6 +12007,12 @@
     <mergeCell ref="B104:D104"/>
     <mergeCell ref="B111:D111"/>
     <mergeCell ref="B118:D118"/>
+    <mergeCell ref="B73:D73"/>
+    <mergeCell ref="B3:C4"/>
+    <mergeCell ref="D3:O3"/>
+    <mergeCell ref="B48:O48"/>
+    <mergeCell ref="B49:C50"/>
+    <mergeCell ref="D49:O49"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -12020,7 +12023,7 @@
   <dimension ref="A2:D23"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -12030,111 +12033,114 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="126" t="s">
+      <c r="A2" s="110" t="s">
         <v>149</v>
       </c>
-      <c r="B2" s="127" t="s">
+      <c r="B2" s="111" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="128">
+      <c r="A3" s="112">
         <v>1</v>
       </c>
-      <c r="B3" s="131" t="s">
+      <c r="B3" s="115" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="129">
+      <c r="A4" s="113">
         <v>2</v>
       </c>
-      <c r="B4" s="132" t="s">
+      <c r="B4" s="116" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="129">
+      <c r="A5" s="113">
         <v>3</v>
       </c>
-      <c r="B5" s="132" t="s">
+      <c r="B5" s="116" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="129">
+      <c r="A6" s="113">
         <v>4</v>
       </c>
-      <c r="B6" s="132" t="s">
+      <c r="B6" s="116" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="129">
-        <v>5</v>
-      </c>
-      <c r="B7" s="132" t="s">
+      <c r="A7" s="113">
+        <v>5</v>
+      </c>
+      <c r="B7" s="116" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="129">
+      <c r="A8" s="113">
         <v>6</v>
       </c>
-      <c r="B8" s="132" t="s">
+      <c r="B8" s="116" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="129">
+      <c r="A9" s="113">
         <v>7</v>
       </c>
-      <c r="B9" s="132" t="s">
+      <c r="B9" s="116" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="129">
+      <c r="A10" s="113">
         <v>8</v>
       </c>
-      <c r="B10" s="132" t="s">
+      <c r="B10" s="116" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="129">
+      <c r="A11" s="113">
         <v>9</v>
       </c>
-      <c r="B11" s="132" t="s">
+      <c r="B11" s="116" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="129">
+      <c r="A12" s="113">
         <v>10</v>
       </c>
-      <c r="B12" s="132" t="s">
+      <c r="B12" s="116" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="129">
+      <c r="A13" s="113">
         <v>11</v>
       </c>
-      <c r="B13" s="132" t="s">
+      <c r="B13" s="116" t="s">
         <v>150</v>
       </c>
+      <c r="C13" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="130">
+      <c r="A14" s="114">
         <v>12</v>
       </c>
-      <c r="B14" s="133" t="s">
+      <c r="B14" s="117" t="s">
         <v>151</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="D15" s="125"/>
+      <c r="D15" s="109"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="D16" s="94"/>
@@ -12193,28 +12199,28 @@
     </row>
     <row r="2" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B3" s="112" t="s">
+      <c r="B3" s="125" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="113"/>
-      <c r="D3" s="109" t="s">
+      <c r="C3" s="126"/>
+      <c r="D3" s="123" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="110"/>
-      <c r="F3" s="110"/>
-      <c r="G3" s="110"/>
-      <c r="H3" s="110"/>
-      <c r="I3" s="110"/>
-      <c r="J3" s="110"/>
-      <c r="K3" s="110"/>
-      <c r="L3" s="110"/>
-      <c r="M3" s="110"/>
-      <c r="N3" s="110"/>
-      <c r="O3" s="111"/>
+      <c r="E3" s="118"/>
+      <c r="F3" s="118"/>
+      <c r="G3" s="118"/>
+      <c r="H3" s="118"/>
+      <c r="I3" s="118"/>
+      <c r="J3" s="118"/>
+      <c r="K3" s="118"/>
+      <c r="L3" s="118"/>
+      <c r="M3" s="118"/>
+      <c r="N3" s="118"/>
+      <c r="O3" s="124"/>
     </row>
     <row r="4" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="114"/>
-      <c r="C4" s="115"/>
+      <c r="B4" s="127"/>
+      <c r="C4" s="128"/>
       <c r="D4" s="23">
         <v>1</v>
       </c>
@@ -14120,46 +14126,46 @@
     </row>
     <row r="47" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="48" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="116" t="s">
+      <c r="B48" s="119" t="s">
         <v>47</v>
       </c>
-      <c r="C48" s="117"/>
-      <c r="D48" s="117"/>
-      <c r="E48" s="117"/>
-      <c r="F48" s="117"/>
-      <c r="G48" s="117"/>
-      <c r="H48" s="117"/>
-      <c r="I48" s="117"/>
-      <c r="J48" s="117"/>
-      <c r="K48" s="117"/>
-      <c r="L48" s="117"/>
-      <c r="M48" s="117"/>
-      <c r="N48" s="117"/>
-      <c r="O48" s="118"/>
+      <c r="C48" s="120"/>
+      <c r="D48" s="120"/>
+      <c r="E48" s="120"/>
+      <c r="F48" s="120"/>
+      <c r="G48" s="120"/>
+      <c r="H48" s="120"/>
+      <c r="I48" s="120"/>
+      <c r="J48" s="120"/>
+      <c r="K48" s="120"/>
+      <c r="L48" s="120"/>
+      <c r="M48" s="120"/>
+      <c r="N48" s="120"/>
+      <c r="O48" s="121"/>
     </row>
     <row r="49" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B49" s="112" t="s">
+      <c r="B49" s="125" t="s">
         <v>0</v>
       </c>
-      <c r="C49" s="113"/>
-      <c r="D49" s="109" t="s">
+      <c r="C49" s="126"/>
+      <c r="D49" s="123" t="s">
         <v>4</v>
       </c>
-      <c r="E49" s="110"/>
-      <c r="F49" s="110"/>
-      <c r="G49" s="110"/>
-      <c r="H49" s="110"/>
-      <c r="I49" s="110"/>
-      <c r="J49" s="110"/>
-      <c r="K49" s="110"/>
-      <c r="L49" s="110"/>
-      <c r="M49" s="110"/>
-      <c r="N49" s="110"/>
-      <c r="O49" s="111"/>
+      <c r="E49" s="118"/>
+      <c r="F49" s="118"/>
+      <c r="G49" s="118"/>
+      <c r="H49" s="118"/>
+      <c r="I49" s="118"/>
+      <c r="J49" s="118"/>
+      <c r="K49" s="118"/>
+      <c r="L49" s="118"/>
+      <c r="M49" s="118"/>
+      <c r="N49" s="118"/>
+      <c r="O49" s="124"/>
     </row>
     <row r="50" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="114"/>
-      <c r="C50" s="115"/>
+      <c r="B50" s="127"/>
+      <c r="C50" s="128"/>
       <c r="D50" s="23">
         <v>1</v>
       </c>
@@ -14823,11 +14829,11 @@
     </row>
     <row r="72" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="73" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="116" t="s">
+      <c r="B73" s="119" t="s">
         <v>61</v>
       </c>
-      <c r="C73" s="117"/>
-      <c r="D73" s="118"/>
+      <c r="C73" s="120"/>
+      <c r="D73" s="121"/>
     </row>
     <row r="74" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B74" s="15">
@@ -14949,11 +14955,11 @@
       </c>
     </row>
     <row r="85" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B85" s="119" t="s">
+      <c r="B85" s="122" t="s">
         <v>62</v>
       </c>
-      <c r="C85" s="119"/>
-      <c r="D85" s="119"/>
+      <c r="C85" s="122"/>
+      <c r="D85" s="122"/>
     </row>
     <row r="86" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="87" spans="2:4" x14ac:dyDescent="0.2">
@@ -15033,11 +15039,11 @@
     </row>
     <row r="94" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="95" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B95" s="109" t="s">
+      <c r="B95" s="123" t="s">
         <v>80</v>
       </c>
-      <c r="C95" s="110"/>
-      <c r="D95" s="111"/>
+      <c r="C95" s="118"/>
+      <c r="D95" s="124"/>
     </row>
     <row r="96" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B96" s="15">
@@ -15104,19 +15110,19 @@
       </c>
     </row>
     <row r="102" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B102" s="110" t="s">
+      <c r="B102" s="118" t="s">
         <v>86</v>
       </c>
-      <c r="C102" s="110"/>
-      <c r="D102" s="110"/>
+      <c r="C102" s="118"/>
+      <c r="D102" s="118"/>
     </row>
     <row r="103" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="104" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B104" s="109" t="s">
+      <c r="B104" s="123" t="s">
         <v>88</v>
       </c>
-      <c r="C104" s="110"/>
-      <c r="D104" s="111"/>
+      <c r="C104" s="118"/>
+      <c r="D104" s="124"/>
     </row>
     <row r="105" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B105" s="15">
@@ -15173,11 +15179,11 @@
     </row>
     <row r="110" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="111" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B111" s="109" t="s">
+      <c r="B111" s="123" t="s">
         <v>93</v>
       </c>
-      <c r="C111" s="110"/>
-      <c r="D111" s="111"/>
+      <c r="C111" s="118"/>
+      <c r="D111" s="124"/>
     </row>
     <row r="112" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B112" s="15">
@@ -15244,19 +15250,19 @@
       </c>
     </row>
     <row r="118" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B118" s="110" t="s">
+      <c r="B118" s="118" t="s">
         <v>99</v>
       </c>
-      <c r="C118" s="110"/>
-      <c r="D118" s="110"/>
+      <c r="C118" s="118"/>
+      <c r="D118" s="118"/>
     </row>
     <row r="119" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="120" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B120" s="116" t="s">
+      <c r="B120" s="119" t="s">
         <v>100</v>
       </c>
-      <c r="C120" s="117"/>
-      <c r="D120" s="118"/>
+      <c r="C120" s="120"/>
+      <c r="D120" s="121"/>
     </row>
     <row r="121" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B121" s="15">
@@ -15511,11 +15517,11 @@
     </row>
     <row r="144" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="145" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B145" s="116" t="s">
+      <c r="B145" s="119" t="s">
         <v>124</v>
       </c>
-      <c r="C145" s="117"/>
-      <c r="D145" s="118"/>
+      <c r="C145" s="120"/>
+      <c r="D145" s="121"/>
     </row>
     <row r="146" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B146" s="15">
@@ -15561,11 +15567,11 @@
     </row>
     <row r="150" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="151" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B151" s="116" t="s">
+      <c r="B151" s="119" t="s">
         <v>128</v>
       </c>
-      <c r="C151" s="117"/>
-      <c r="D151" s="118"/>
+      <c r="C151" s="120"/>
+      <c r="D151" s="121"/>
     </row>
     <row r="152" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B152" s="15">
@@ -15599,12 +15605,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B73:D73"/>
-    <mergeCell ref="B3:C4"/>
-    <mergeCell ref="D3:O3"/>
-    <mergeCell ref="B48:O48"/>
-    <mergeCell ref="B49:C50"/>
-    <mergeCell ref="D49:O49"/>
     <mergeCell ref="B120:D120"/>
     <mergeCell ref="B145:D145"/>
     <mergeCell ref="B151:D151"/>
@@ -15614,6 +15614,12 @@
     <mergeCell ref="B104:D104"/>
     <mergeCell ref="B111:D111"/>
     <mergeCell ref="B118:D118"/>
+    <mergeCell ref="B73:D73"/>
+    <mergeCell ref="B3:C4"/>
+    <mergeCell ref="D3:O3"/>
+    <mergeCell ref="B48:O48"/>
+    <mergeCell ref="B49:C50"/>
+    <mergeCell ref="D49:O49"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -15644,28 +15650,28 @@
     </row>
     <row r="2" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B3" s="112" t="s">
+      <c r="B3" s="125" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="113"/>
-      <c r="D3" s="109" t="s">
+      <c r="C3" s="126"/>
+      <c r="D3" s="123" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="110"/>
-      <c r="F3" s="110"/>
-      <c r="G3" s="110"/>
-      <c r="H3" s="110"/>
-      <c r="I3" s="110"/>
-      <c r="J3" s="110"/>
-      <c r="K3" s="110"/>
-      <c r="L3" s="110"/>
-      <c r="M3" s="110"/>
-      <c r="N3" s="110"/>
-      <c r="O3" s="111"/>
+      <c r="E3" s="118"/>
+      <c r="F3" s="118"/>
+      <c r="G3" s="118"/>
+      <c r="H3" s="118"/>
+      <c r="I3" s="118"/>
+      <c r="J3" s="118"/>
+      <c r="K3" s="118"/>
+      <c r="L3" s="118"/>
+      <c r="M3" s="118"/>
+      <c r="N3" s="118"/>
+      <c r="O3" s="124"/>
     </row>
     <row r="4" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="114"/>
-      <c r="C4" s="115"/>
+      <c r="B4" s="127"/>
+      <c r="C4" s="128"/>
       <c r="D4" s="23">
         <v>1</v>
       </c>
@@ -17571,46 +17577,46 @@
     </row>
     <row r="47" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="48" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="116" t="s">
+      <c r="B48" s="119" t="s">
         <v>47</v>
       </c>
-      <c r="C48" s="117"/>
-      <c r="D48" s="117"/>
-      <c r="E48" s="117"/>
-      <c r="F48" s="117"/>
-      <c r="G48" s="117"/>
-      <c r="H48" s="117"/>
-      <c r="I48" s="117"/>
-      <c r="J48" s="117"/>
-      <c r="K48" s="117"/>
-      <c r="L48" s="117"/>
-      <c r="M48" s="117"/>
-      <c r="N48" s="117"/>
-      <c r="O48" s="118"/>
+      <c r="C48" s="120"/>
+      <c r="D48" s="120"/>
+      <c r="E48" s="120"/>
+      <c r="F48" s="120"/>
+      <c r="G48" s="120"/>
+      <c r="H48" s="120"/>
+      <c r="I48" s="120"/>
+      <c r="J48" s="120"/>
+      <c r="K48" s="120"/>
+      <c r="L48" s="120"/>
+      <c r="M48" s="120"/>
+      <c r="N48" s="120"/>
+      <c r="O48" s="121"/>
     </row>
     <row r="49" spans="2:15" x14ac:dyDescent="0.2">
-      <c r="B49" s="112" t="s">
+      <c r="B49" s="125" t="s">
         <v>0</v>
       </c>
-      <c r="C49" s="113"/>
-      <c r="D49" s="109" t="s">
+      <c r="C49" s="126"/>
+      <c r="D49" s="123" t="s">
         <v>4</v>
       </c>
-      <c r="E49" s="110"/>
-      <c r="F49" s="110"/>
-      <c r="G49" s="110"/>
-      <c r="H49" s="110"/>
-      <c r="I49" s="110"/>
-      <c r="J49" s="110"/>
-      <c r="K49" s="110"/>
-      <c r="L49" s="110"/>
-      <c r="M49" s="110"/>
-      <c r="N49" s="110"/>
-      <c r="O49" s="111"/>
+      <c r="E49" s="118"/>
+      <c r="F49" s="118"/>
+      <c r="G49" s="118"/>
+      <c r="H49" s="118"/>
+      <c r="I49" s="118"/>
+      <c r="J49" s="118"/>
+      <c r="K49" s="118"/>
+      <c r="L49" s="118"/>
+      <c r="M49" s="118"/>
+      <c r="N49" s="118"/>
+      <c r="O49" s="124"/>
     </row>
     <row r="50" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="114"/>
-      <c r="C50" s="115"/>
+      <c r="B50" s="127"/>
+      <c r="C50" s="128"/>
       <c r="D50" s="23">
         <v>1</v>
       </c>
@@ -18274,11 +18280,11 @@
     </row>
     <row r="72" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="73" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="116" t="s">
+      <c r="B73" s="119" t="s">
         <v>61</v>
       </c>
-      <c r="C73" s="117"/>
-      <c r="D73" s="118"/>
+      <c r="C73" s="120"/>
+      <c r="D73" s="121"/>
     </row>
     <row r="74" spans="2:15" x14ac:dyDescent="0.2">
       <c r="B74" s="15">
@@ -18400,11 +18406,11 @@
       </c>
     </row>
     <row r="85" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B85" s="119" t="s">
+      <c r="B85" s="122" t="s">
         <v>62</v>
       </c>
-      <c r="C85" s="119"/>
-      <c r="D85" s="119"/>
+      <c r="C85" s="122"/>
+      <c r="D85" s="122"/>
     </row>
     <row r="86" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="87" spans="2:4" x14ac:dyDescent="0.2">
@@ -18484,11 +18490,11 @@
     </row>
     <row r="94" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="95" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B95" s="109" t="s">
+      <c r="B95" s="123" t="s">
         <v>80</v>
       </c>
-      <c r="C95" s="110"/>
-      <c r="D95" s="111"/>
+      <c r="C95" s="118"/>
+      <c r="D95" s="124"/>
     </row>
     <row r="96" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B96" s="15">
@@ -18555,19 +18561,19 @@
       </c>
     </row>
     <row r="102" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B102" s="110" t="s">
+      <c r="B102" s="118" t="s">
         <v>86</v>
       </c>
-      <c r="C102" s="110"/>
-      <c r="D102" s="110"/>
+      <c r="C102" s="118"/>
+      <c r="D102" s="118"/>
     </row>
     <row r="103" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="104" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B104" s="109" t="s">
+      <c r="B104" s="123" t="s">
         <v>88</v>
       </c>
-      <c r="C104" s="110"/>
-      <c r="D104" s="111"/>
+      <c r="C104" s="118"/>
+      <c r="D104" s="124"/>
     </row>
     <row r="105" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B105" s="15">
@@ -18624,11 +18630,11 @@
     </row>
     <row r="110" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="111" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B111" s="109" t="s">
+      <c r="B111" s="123" t="s">
         <v>93</v>
       </c>
-      <c r="C111" s="110"/>
-      <c r="D111" s="111"/>
+      <c r="C111" s="118"/>
+      <c r="D111" s="124"/>
     </row>
     <row r="112" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B112" s="15">
@@ -18695,19 +18701,19 @@
       </c>
     </row>
     <row r="118" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B118" s="110" t="s">
+      <c r="B118" s="118" t="s">
         <v>99</v>
       </c>
-      <c r="C118" s="110"/>
-      <c r="D118" s="110"/>
+      <c r="C118" s="118"/>
+      <c r="D118" s="118"/>
     </row>
     <row r="119" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="120" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B120" s="116" t="s">
+      <c r="B120" s="119" t="s">
         <v>100</v>
       </c>
-      <c r="C120" s="117"/>
-      <c r="D120" s="118"/>
+      <c r="C120" s="120"/>
+      <c r="D120" s="121"/>
     </row>
     <row r="121" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B121" s="15">
@@ -18962,11 +18968,11 @@
     </row>
     <row r="144" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="145" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B145" s="116" t="s">
+      <c r="B145" s="119" t="s">
         <v>124</v>
       </c>
-      <c r="C145" s="117"/>
-      <c r="D145" s="118"/>
+      <c r="C145" s="120"/>
+      <c r="D145" s="121"/>
     </row>
     <row r="146" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B146" s="15">
@@ -19012,11 +19018,11 @@
     </row>
     <row r="150" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="151" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B151" s="116" t="s">
+      <c r="B151" s="119" t="s">
         <v>128</v>
       </c>
-      <c r="C151" s="117"/>
-      <c r="D151" s="118"/>
+      <c r="C151" s="120"/>
+      <c r="D151" s="121"/>
     </row>
     <row r="152" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B152" s="15">
@@ -19050,12 +19056,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B73:D73"/>
-    <mergeCell ref="B3:C4"/>
-    <mergeCell ref="D3:O3"/>
-    <mergeCell ref="B48:O48"/>
-    <mergeCell ref="B49:C50"/>
-    <mergeCell ref="D49:O49"/>
     <mergeCell ref="B120:D120"/>
     <mergeCell ref="B145:D145"/>
     <mergeCell ref="B151:D151"/>
@@ -19065,6 +19065,12 @@
     <mergeCell ref="B104:D104"/>
     <mergeCell ref="B111:D111"/>
     <mergeCell ref="B118:D118"/>
+    <mergeCell ref="B73:D73"/>
+    <mergeCell ref="B3:C4"/>
+    <mergeCell ref="D3:O3"/>
+    <mergeCell ref="B48:O48"/>
+    <mergeCell ref="B49:C50"/>
+    <mergeCell ref="D49:O49"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -19095,21 +19101,21 @@
       <c r="A2" s="106"/>
     </row>
     <row r="3" spans="1:13" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="123" t="s">
+      <c r="A3" s="132" t="s">
         <v>144</v>
       </c>
-      <c r="B3" s="123"/>
-      <c r="C3" s="123"/>
-      <c r="D3" s="123"/>
-      <c r="E3" s="123"/>
-      <c r="F3" s="123"/>
-      <c r="G3" s="123"/>
-      <c r="H3" s="123"/>
-      <c r="I3" s="123"/>
-      <c r="J3" s="123"/>
-      <c r="K3" s="123"/>
-      <c r="L3" s="123"/>
-      <c r="M3" s="123"/>
+      <c r="B3" s="132"/>
+      <c r="C3" s="132"/>
+      <c r="D3" s="132"/>
+      <c r="E3" s="132"/>
+      <c r="F3" s="132"/>
+      <c r="G3" s="132"/>
+      <c r="H3" s="132"/>
+      <c r="I3" s="132"/>
+      <c r="J3" s="132"/>
+      <c r="K3" s="132"/>
+      <c r="L3" s="132"/>
+      <c r="M3" s="132"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="104"/>
@@ -19123,61 +19129,61 @@
       <c r="A6" s="106"/>
     </row>
     <row r="7" spans="1:13" s="107" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="123" t="s">
+      <c r="A7" s="132" t="s">
         <v>146</v>
       </c>
-      <c r="B7" s="123"/>
-      <c r="C7" s="123"/>
-      <c r="D7" s="123"/>
-      <c r="E7" s="123"/>
-      <c r="F7" s="123"/>
-      <c r="G7" s="123"/>
-      <c r="H7" s="123"/>
-      <c r="I7" s="123"/>
-      <c r="J7" s="123"/>
-      <c r="K7" s="123"/>
-      <c r="L7" s="123"/>
-      <c r="M7" s="123"/>
+      <c r="B7" s="132"/>
+      <c r="C7" s="132"/>
+      <c r="D7" s="132"/>
+      <c r="E7" s="132"/>
+      <c r="F7" s="132"/>
+      <c r="G7" s="132"/>
+      <c r="H7" s="132"/>
+      <c r="I7" s="132"/>
+      <c r="J7" s="132"/>
+      <c r="K7" s="132"/>
+      <c r="L7" s="132"/>
+      <c r="M7" s="132"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" s="106"/>
     </row>
     <row r="9" spans="1:13" ht="99" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="123" t="s">
+      <c r="A9" s="132" t="s">
         <v>147</v>
       </c>
-      <c r="B9" s="123"/>
-      <c r="C9" s="123"/>
-      <c r="D9" s="123"/>
-      <c r="E9" s="123"/>
-      <c r="F9" s="123"/>
-      <c r="G9" s="123"/>
-      <c r="H9" s="123"/>
-      <c r="I9" s="123"/>
-      <c r="J9" s="123"/>
-      <c r="K9" s="123"/>
-      <c r="L9" s="123"/>
-      <c r="M9" s="123"/>
+      <c r="B9" s="132"/>
+      <c r="C9" s="132"/>
+      <c r="D9" s="132"/>
+      <c r="E9" s="132"/>
+      <c r="F9" s="132"/>
+      <c r="G9" s="132"/>
+      <c r="H9" s="132"/>
+      <c r="I9" s="132"/>
+      <c r="J9" s="132"/>
+      <c r="K9" s="132"/>
+      <c r="L9" s="132"/>
+      <c r="M9" s="132"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="104"/>
     </row>
     <row r="11" spans="1:13" ht="32" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="123" t="s">
+      <c r="A11" s="132" t="s">
         <v>145</v>
       </c>
-      <c r="B11" s="123"/>
-      <c r="C11" s="123"/>
-      <c r="D11" s="123"/>
-      <c r="E11" s="123"/>
-      <c r="F11" s="123"/>
-      <c r="G11" s="123"/>
-      <c r="H11" s="123"/>
-      <c r="I11" s="123"/>
-      <c r="J11" s="123"/>
-      <c r="K11" s="123"/>
-      <c r="L11" s="123"/>
-      <c r="M11" s="123"/>
+      <c r="B11" s="132"/>
+      <c r="C11" s="132"/>
+      <c r="D11" s="132"/>
+      <c r="E11" s="132"/>
+      <c r="F11" s="132"/>
+      <c r="G11" s="132"/>
+      <c r="H11" s="132"/>
+      <c r="I11" s="132"/>
+      <c r="J11" s="132"/>
+      <c r="K11" s="132"/>
+      <c r="L11" s="132"/>
+      <c r="M11" s="132"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" s="94"/>
@@ -19190,20 +19196,20 @@
     <row r="14" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="46"/>
-      <c r="B15" s="109" t="s">
+      <c r="B15" s="123" t="s">
         <v>4</v>
       </c>
-      <c r="C15" s="110"/>
-      <c r="D15" s="110"/>
-      <c r="E15" s="110"/>
-      <c r="F15" s="110"/>
-      <c r="G15" s="110"/>
-      <c r="H15" s="110"/>
-      <c r="I15" s="110"/>
-      <c r="J15" s="110"/>
-      <c r="K15" s="110"/>
-      <c r="L15" s="110"/>
-      <c r="M15" s="111"/>
+      <c r="C15" s="118"/>
+      <c r="D15" s="118"/>
+      <c r="E15" s="118"/>
+      <c r="F15" s="118"/>
+      <c r="G15" s="118"/>
+      <c r="H15" s="118"/>
+      <c r="I15" s="118"/>
+      <c r="J15" s="118"/>
+      <c r="K15" s="118"/>
+      <c r="L15" s="118"/>
+      <c r="M15" s="124"/>
     </row>
     <row r="16" spans="1:13" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="51" t="s">
@@ -19542,28 +19548,28 @@
     </row>
     <row r="2" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="2:17" x14ac:dyDescent="0.2">
-      <c r="B3" s="112" t="s">
+      <c r="B3" s="125" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="113"/>
-      <c r="D3" s="109" t="s">
+      <c r="C3" s="126"/>
+      <c r="D3" s="123" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="110"/>
-      <c r="F3" s="110"/>
-      <c r="G3" s="110"/>
-      <c r="H3" s="110"/>
-      <c r="I3" s="110"/>
-      <c r="J3" s="110"/>
-      <c r="K3" s="110"/>
-      <c r="L3" s="110"/>
-      <c r="M3" s="110"/>
-      <c r="N3" s="110"/>
-      <c r="O3" s="111"/>
+      <c r="E3" s="118"/>
+      <c r="F3" s="118"/>
+      <c r="G3" s="118"/>
+      <c r="H3" s="118"/>
+      <c r="I3" s="118"/>
+      <c r="J3" s="118"/>
+      <c r="K3" s="118"/>
+      <c r="L3" s="118"/>
+      <c r="M3" s="118"/>
+      <c r="N3" s="118"/>
+      <c r="O3" s="124"/>
     </row>
     <row r="4" spans="2:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="114"/>
-      <c r="C4" s="115"/>
+      <c r="B4" s="127"/>
+      <c r="C4" s="128"/>
       <c r="D4" s="23">
         <v>1</v>
       </c>
@@ -21468,46 +21474,46 @@
       <c r="Q46" s="1"/>
     </row>
     <row r="48" spans="2:17" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="116" t="s">
+      <c r="B48" s="119" t="s">
         <v>47</v>
       </c>
-      <c r="C48" s="117"/>
-      <c r="D48" s="117"/>
-      <c r="E48" s="117"/>
-      <c r="F48" s="117"/>
-      <c r="G48" s="117"/>
-      <c r="H48" s="117"/>
-      <c r="I48" s="117"/>
-      <c r="J48" s="117"/>
-      <c r="K48" s="117"/>
-      <c r="L48" s="117"/>
-      <c r="M48" s="117"/>
-      <c r="N48" s="117"/>
-      <c r="O48" s="118"/>
+      <c r="C48" s="120"/>
+      <c r="D48" s="120"/>
+      <c r="E48" s="120"/>
+      <c r="F48" s="120"/>
+      <c r="G48" s="120"/>
+      <c r="H48" s="120"/>
+      <c r="I48" s="120"/>
+      <c r="J48" s="120"/>
+      <c r="K48" s="120"/>
+      <c r="L48" s="120"/>
+      <c r="M48" s="120"/>
+      <c r="N48" s="120"/>
+      <c r="O48" s="121"/>
     </row>
     <row r="49" spans="2:15" hidden="1" x14ac:dyDescent="0.2">
-      <c r="B49" s="112" t="s">
+      <c r="B49" s="125" t="s">
         <v>0</v>
       </c>
-      <c r="C49" s="113"/>
-      <c r="D49" s="109" t="s">
+      <c r="C49" s="126"/>
+      <c r="D49" s="123" t="s">
         <v>4</v>
       </c>
-      <c r="E49" s="110"/>
-      <c r="F49" s="110"/>
-      <c r="G49" s="110"/>
-      <c r="H49" s="110"/>
-      <c r="I49" s="110"/>
-      <c r="J49" s="110"/>
-      <c r="K49" s="110"/>
-      <c r="L49" s="110"/>
-      <c r="M49" s="110"/>
-      <c r="N49" s="110"/>
-      <c r="O49" s="111"/>
+      <c r="E49" s="118"/>
+      <c r="F49" s="118"/>
+      <c r="G49" s="118"/>
+      <c r="H49" s="118"/>
+      <c r="I49" s="118"/>
+      <c r="J49" s="118"/>
+      <c r="K49" s="118"/>
+      <c r="L49" s="118"/>
+      <c r="M49" s="118"/>
+      <c r="N49" s="118"/>
+      <c r="O49" s="124"/>
     </row>
     <row r="50" spans="2:15" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B50" s="114"/>
-      <c r="C50" s="115"/>
+      <c r="B50" s="127"/>
+      <c r="C50" s="128"/>
       <c r="D50" s="23">
         <v>1</v>
       </c>
@@ -22171,11 +22177,11 @@
     </row>
     <row r="72" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="73" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B73" s="116" t="s">
+      <c r="B73" s="119" t="s">
         <v>61</v>
       </c>
-      <c r="C73" s="117"/>
-      <c r="D73" s="118"/>
+      <c r="C73" s="120"/>
+      <c r="D73" s="121"/>
     </row>
     <row r="74" spans="2:15" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B74" s="15">
@@ -22297,11 +22303,11 @@
       </c>
     </row>
     <row r="85" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B85" s="124" t="s">
+      <c r="B85" s="133" t="s">
         <v>62</v>
       </c>
-      <c r="C85" s="124"/>
-      <c r="D85" s="124"/>
+      <c r="C85" s="133"/>
+      <c r="D85" s="133"/>
     </row>
     <row r="87" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B87" s="15">
@@ -22380,11 +22386,11 @@
     </row>
     <row r="94" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="95" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B95" s="109" t="s">
+      <c r="B95" s="123" t="s">
         <v>80</v>
       </c>
-      <c r="C95" s="110"/>
-      <c r="D95" s="111"/>
+      <c r="C95" s="118"/>
+      <c r="D95" s="124"/>
     </row>
     <row r="96" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B96" s="15">
@@ -22451,18 +22457,18 @@
       </c>
     </row>
     <row r="102" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B102" s="121" t="s">
+      <c r="B102" s="130" t="s">
         <v>86</v>
       </c>
-      <c r="C102" s="121"/>
-      <c r="D102" s="121"/>
+      <c r="C102" s="130"/>
+      <c r="D102" s="130"/>
     </row>
     <row r="104" spans="2:4" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B104" s="109" t="s">
+      <c r="B104" s="123" t="s">
         <v>88</v>
       </c>
-      <c r="C104" s="110"/>
-      <c r="D104" s="111"/>
+      <c r="C104" s="118"/>
+      <c r="D104" s="124"/>
     </row>
     <row r="105" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B105" s="15">
@@ -22519,11 +22525,11 @@
     </row>
     <row r="110" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="111" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B111" s="109" t="s">
+      <c r="B111" s="123" t="s">
         <v>93</v>
       </c>
-      <c r="C111" s="110"/>
-      <c r="D111" s="111"/>
+      <c r="C111" s="118"/>
+      <c r="D111" s="124"/>
     </row>
     <row r="112" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B112" s="15">
@@ -22590,18 +22596,18 @@
       </c>
     </row>
     <row r="118" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B118" s="121" t="s">
+      <c r="B118" s="130" t="s">
         <v>99</v>
       </c>
-      <c r="C118" s="121"/>
-      <c r="D118" s="121"/>
+      <c r="C118" s="130"/>
+      <c r="D118" s="130"/>
     </row>
     <row r="120" spans="2:4" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B120" s="116" t="s">
+      <c r="B120" s="119" t="s">
         <v>100</v>
       </c>
-      <c r="C120" s="117"/>
-      <c r="D120" s="118"/>
+      <c r="C120" s="120"/>
+      <c r="D120" s="121"/>
     </row>
     <row r="121" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B121" s="15">
@@ -22856,11 +22862,11 @@
     </row>
     <row r="144" spans="2:4" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="145" spans="2:4" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B145" s="116" t="s">
+      <c r="B145" s="119" t="s">
         <v>124</v>
       </c>
-      <c r="C145" s="117"/>
-      <c r="D145" s="118"/>
+      <c r="C145" s="120"/>
+      <c r="D145" s="121"/>
     </row>
     <row r="146" spans="2:4" hidden="1" x14ac:dyDescent="0.2">
       <c r="B146" s="15">
@@ -22906,11 +22912,11 @@
     </row>
     <row r="150" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="151" spans="2:4" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B151" s="116" t="s">
+      <c r="B151" s="119" t="s">
         <v>128</v>
       </c>
-      <c r="C151" s="117"/>
-      <c r="D151" s="118"/>
+      <c r="C151" s="120"/>
+      <c r="D151" s="121"/>
     </row>
     <row r="152" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B152" s="15">
@@ -22944,12 +22950,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="B73:D73"/>
-    <mergeCell ref="B3:C4"/>
-    <mergeCell ref="D3:O3"/>
-    <mergeCell ref="B48:O48"/>
-    <mergeCell ref="B49:C50"/>
-    <mergeCell ref="D49:O49"/>
     <mergeCell ref="B120:D120"/>
     <mergeCell ref="B145:D145"/>
     <mergeCell ref="B151:D151"/>
@@ -22959,6 +22959,12 @@
     <mergeCell ref="B104:D104"/>
     <mergeCell ref="B111:D111"/>
     <mergeCell ref="B118:D118"/>
+    <mergeCell ref="B73:D73"/>
+    <mergeCell ref="B3:C4"/>
+    <mergeCell ref="D3:O3"/>
+    <mergeCell ref="B48:O48"/>
+    <mergeCell ref="B49:C50"/>
+    <mergeCell ref="D49:O49"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>